<commit_message>
new Calc week Statistic
</commit_message>
<xml_diff>
--- a/ProcessingCheckListWss/bin/Debug/Result/Возражения.xlsx
+++ b/ProcessingCheckListWss/bin/Debug/Result/Возражения.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <x:si>
-    <x:t>Возражения по звонкам с 25.06 по 01.07</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <x:si>
+    <x:t>Возражения по звонкам с 01.07 по 14.07</x:t>
   </x:si>
   <x:si>
     <x:t>Менеджер</x:t>
@@ -37,112 +37,76 @@
     <x:t>Результат</x:t>
   </x:si>
   <x:si>
-    <x:t>Владимир</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 473 239-16-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29.06.2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Не используют такие виды полов, так как дорого</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложил КП для сравнения. Сказал, что конкурируют с европейским аналогом</x:t>
-  </x:si>
-  <x:si>
-    <x:t>В работе</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Мхитар</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 383 262-99-33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26.06.2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Возражения со стороны секретаря. Отказалась давать данные директора</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Менеджер попытался объяснить, что для того, чтобы отправить КП, необходимо задать несколько вопросов директору.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 423 240-67-40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25.06.2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Изначально у клиента не было интереса</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Рассказал о технологии нанесения напольного покрытия</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Клиента смущает, что компания находится в Иваново.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Менеджер сказал, что работают по всей России. Есть партнеры и подрядчики.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 395 233-56-11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Все работы уже закончили. Покрытие клиента устраивает, другое не интересно.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Рассказал о покрытии (долго служит и тп). Отправил клиенту вводную информацию.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 383 210-51-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Клиент не хочет предоставить менеджеру документацию для расчета.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Менеджер объяснил, что это необходимо для более подробной информации. Менеджеру необходимо более уверенно работать с возражениями.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 347 237-02-08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Клиент попросил предложение с составом и стоимостью квадратного метра. Дополнительной информации менеджеру не предоставил.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Менеджер сказал, что необходимо составить ТЗ, для этого необходима дополнительная информация. Убедить клиента не получилось.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Татьяна</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 391 204-14-70</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Клиент использует линолеум и сомневается стоит ли менять или нет.</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Рассказала о преимуществах полиуретанового покрытия. </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 347 983-31-04</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Хочет знать стоимость. Несколько раз менял покрытия. Сейчас есть образцы от других компаний.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Рассказала о преимуществах напольного покрытия, о том, что устойчиво к любым химическим воздействиям и тп.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на +7 817 382-31-18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Клиенту необходимо знать стоимость на дополнительные работы</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Менеджер объяснила, что дополнительные работы рассчитываются индивидуально. Уточнит у экспертов и свяжется с клиентом.</x:t>
+    <x:t>Шутова</x:t>
+  </x:si>
+  <x:si>
+    <x:t>02.07.2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Купил</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Менеджер поинтересовался у клиент  где купил, кто производитель</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Упущена</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03.07.2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Дорого</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Клиент оставив запрос, написал комментарий. Менеджер объяснила, что ничего не отобразилось. Работать с возражениями клиента у менеджера не было возможности, клиент сказал не беспокоить его.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Клиенту не подходит размер</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Менеджер выяснил причину отказа</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Купили в другой компании</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Купили, неактуально</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Щетинина</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09.07.2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Купил в другой компании</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Менеджер не смог предложить другой вариант т.к. клиент уже купил.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Янина</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08.07.2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Для клиента дорого</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Менеджер предложил другие варианты, более дешевые по стоимости</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Не подходит размер</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Менеджер предложил другой вариант</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Клиент хотел приобрести товар в розницу</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Менеджер выявил потребность</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -152,7 +116,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="3">
+  <x:fonts count="2">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -168,14 +132,6 @@
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
-    <x:font>
-      <x:u val="single"/>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color theme="10"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
   </x:fonts>
   <x:fills count="2">
     <x:fill>
@@ -221,30 +177,23 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="4">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -547,7 +496,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F12"/>
+  <x:dimension ref="A1:F11"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -593,207 +542,177 @@
       <x:c r="A3" s="1" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B3" s="2" t="s">
+      <x:c r="B3" s="2" t="n">
+        <x:v>89049556819</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C3" s="3" t="s">
+      <x:c r="D3" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D3" s="3" t="s">
+      <x:c r="E3" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E3" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="F3" s="3" t="s">
+      <x:c r="F3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="1" t="s"/>
+      <x:c r="B4" s="2" t="n">
+        <x:v>89108248721</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="A4" s="1" t="s">
+      <x:c r="D4" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B4" s="2" t="s">
+      <x:c r="E4" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C4" s="3" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D4" s="3" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="E4" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F4" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="F4" s="2" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="1" t="s"/>
-      <x:c r="B5" s="2" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C5" s="3" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D5" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E5" s="3" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="F5" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="B5" s="2" t="n">
+        <x:v>89162450180</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="1" t="s"/>
-      <x:c r="B6" s="2" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C6" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D6" s="3" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E6" s="3" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="F6" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="B6" s="2" t="n">
+        <x:v>89041668023</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
       <x:c r="A7" s="1" t="s"/>
-      <x:c r="B7" s="2" t="s">
+      <x:c r="B7" s="2" t="n">
+        <x:v>89030350911</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="1" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="n">
+        <x:v>89676680447</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E8" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="n">
+        <x:v>89059994285</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C7" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D7" s="3" t="s">
+      <x:c r="D9" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="E7" s="3" t="s">
+      <x:c r="E9" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="F7" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6">
-      <x:c r="A8" s="1" t="s"/>
-      <x:c r="B8" s="2" t="s">
+      <x:c r="F9" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="1" t="s"/>
+      <x:c r="B10" s="2" t="n">
+        <x:v>89213582332</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C8" s="3" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D8" s="3" t="s">
+      <x:c r="E10" s="2" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="E8" s="3" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="F8" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:6">
-      <x:c r="A9" s="1" t="s"/>
-      <x:c r="B9" s="2" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C9" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D9" s="3" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E9" s="3" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="F9" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:6">
-      <x:c r="A10" s="1" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="B10" s="2" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="C10" s="3" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D10" s="3" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="E10" s="3" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="F10" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="F10" s="2" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="1" t="s"/>
-      <x:c r="B11" s="2" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="C11" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D11" s="3" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E11" s="3" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="F11" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:6">
-      <x:c r="A12" s="1" t="s"/>
-      <x:c r="B12" s="2" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="C12" s="3" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D12" s="3" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="E12" s="3" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="F12" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="B11" s="2" t="n">
+        <x:v>9273575551</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="4">
     <x:mergeCell ref="A1:E1"/>
-    <x:mergeCell ref="A3:A3"/>
-    <x:mergeCell ref="A4:A9"/>
-    <x:mergeCell ref="A10:A12"/>
+    <x:mergeCell ref="A3:A7"/>
+    <x:mergeCell ref="A8:A8"/>
+    <x:mergeCell ref="A9:A11"/>
   </x:mergeCells>
-  <x:hyperlinks>
-    <x:hyperlink ref="B3" r:id="rId5"/>
-    <x:hyperlink ref="B4" r:id="rId6"/>
-    <x:hyperlink ref="B5" r:id="rId7"/>
-    <x:hyperlink ref="B6" r:id="rId8"/>
-    <x:hyperlink ref="B7" r:id="rId9"/>
-    <x:hyperlink ref="B8" r:id="rId10"/>
-    <x:hyperlink ref="B9" r:id="rId11"/>
-    <x:hyperlink ref="B10" r:id="rId12"/>
-    <x:hyperlink ref="B11" r:id="rId13"/>
-    <x:hyperlink ref="B12" r:id="rId14"/>
-  </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>

<commit_message>
fix bug with february
</commit_message>
<xml_diff>
--- a/ProcessingCheckListWss/bin/Debug/Result/Возражения.xlsx
+++ b/ProcessingCheckListWss/bin/Debug/Result/Возражения.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
-  <x:si>
-    <x:t>Возражения по звонкам по 28.02</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+  <x:si>
+    <x:t>Возражения по звонкам по 27.02</x:t>
   </x:si>
   <x:si>
     <x:t>Статистика</x:t>
@@ -221,375 +221,6 @@
   </x:si>
   <x:si>
     <x:t>05.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Борисова</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Заявка на просчёт </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 919 698-70-81</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Квартира еще не куплена</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Приглашение в салон, озвучил преимущества раннего подхода к проекту, согласовал повторную дату звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>03.04.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 8 (963) 157-71-60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиенту не удобно разговаривать.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложен визит в салон, рассказаны преимущества посещения салона, почти согласован визит.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 8 (906) 325-14-45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Кухня не актуальна, интересовала цена.</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Предложено посещение салона, просчет.  </x:t>
-  </x:si>
-  <x:si>
-    <x:t>03.10.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 985 748-57-68</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Вопрос клиента по ранее купленной кухне, по уменьшению размеров.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Выслушал клиента, по вопросу клиента постарался решить вопрос, согласовано перезвонить через минутку, последующего разговора с клиентом нет.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 925 660-02-65</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Интересовал только адрес салона, на просчет и посещения салона точно не решился.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Менеджер ответил на все вопросы клиента. Предложил связь с дизайнером, посещение салона.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 8 (900) 281-52-48</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Приезд в салон не возможен,муж в командировке.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено посещение салона, согласована дата повторного звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20.03.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 962 863-00-60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Не подходит стоимость кухни.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Озвучил ассортимент по цене,  рассрочку, в дальнейшем обратиться повторно.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Рекорд</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 965 400-70-70</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиент интересовался сертификатами, был уже в салоне.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ознакомил с сертификатами, предложил связаться с дизайнером, предложил посетить салон.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 925 877-99-08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Начинается ремонт,  рассматривают варианты кухни.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложен салон, заранее приступить к проекту, озвучены скидки, консультация по БТ, согласована дата повторного звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 906 799-57-99</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Кухня не актуальна.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Нет</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено вручение сертификатов.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 925 311-94-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. По кухне занимается супруга по другому номеру телефона.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Сделал приглашение в салон, предложил просчет, повторный звонок.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 977 705-41-32</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Другое. Прервался разговор. </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложил замер, повторный звонок, рассказал про сертификаты, предложил корпусную мебель.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 926 289-76-92</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиента интересовала БТ, в помещении ремонт.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ответил на все вопросы клиента, предложен салон, замер, согласована дата повторного звонка для уточнения продвижения дел.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 909 975-64-74</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Кухня актуальна через два года, заказ будет делать точно в этой компании.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложил посещение салона, закрепить заявку за дизайнером, озвучена фиксированная цена при заказе.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Гуськова_</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 926 236-18-62</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Клиент подумает, для него дорого.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено посетить салон, просчитать кухню онлайн, подсчитана примерная стоимость, озвучена рассрочка, на дальнейшее предложено оставить заявку на сайте.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 916 858-31-31</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. По кухне решается вопрос с дочерью.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложил выслать номер для связи, перезвонить вечером сам.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 926 998-67-19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиент подумает, мастер приступит к ремонту в марте, повторное общение в марте месяце.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложен предварительный просчет, озвучены скидки, согласована дата повторного звонка в марте месяце.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 925 716-12-60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Кухни неактуальны, интересует шкаф, неудобно продолжать разговор.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложена корпусная мебель, согласована дата повторного звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 905 793-55-09</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиенту не удобно разговаривать, просил позвонить через две недели.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено создать дизайн проект, согласована дата повторного звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11.03.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 916 091-51-13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Желание клиента созвониться в мае.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложил салон, просчет, согласовал дату повторного звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27.05.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 953 966-52-36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Желание клиента созвониться в апреле.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено созвониться напрямую с дочерью, согласована дата повторного звонка в апреле.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01.04.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 912 631-09-50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Не подходит по бюджету.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено создать проект, рассчитана стартовая цена кухни, посоветовал обратиться на сайт при актуальном вопросе.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 977 676-01-47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Не помнит сайт, оставит заявку повторно.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложил рассмотреть сайт и повторно оставить заявку.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 977 707-17-65</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Дорого для клиента.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Посчитал стартовую стоимость</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Упущена</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 977 453-61-22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Желание клиента созвониться в марте.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено создать дизайн проект, выслать каталог, согласована дата повторного звонка.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29.03.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 999 920-99-16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиент сам заедет в салон.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Рассказано про рассрочку, предложен салон, сориентирован по адресу.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Прокофьева</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 921 723-10-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Кухня актуальна, есть интерес поработать с дизайнером, уезжают в отпуск.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено посещение салона, озвучена связь с дизайнером и его работа, согласована дата повторного звонка о уточнения даты посещения салона.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13.03.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Римма</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 985 869-09-18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Клиента не устроила стоимость по просчету дизайнера.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено на месте в салоне поменять проект, сменить материал.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 915 426-51-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Клиент не может определиться с датой посещения, маленький ребенок.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>По кухне диалог состоялся в полном объеме, согласована дата повторного звонка для уточнения даты посещения салона.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 909 998-20-02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Клиента не устроила примерная цена кухни, есть свои понимания.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Предложено посещения салона, онлайн просчет, рассказано про производство компании, при повторном обращении предложено оставить заявку на сайте.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 985 045-00-30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Не актуально.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>При актуальности предложено оставить заявку на сайте.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 7 928 206-55-26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25.02.2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Цена. Клиенту дорого.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Рассказано от чего зависит стоимость кухни, предложен предварительный просчет, при обращении в дальнейшем повторить заявку.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Исходящий на 8 (900) 249-11-98</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Другое. Кухня для детей, клиент мало владеет информацией.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Озвучено преимущество посещения салона, согласована дата повторного звонка разговора с непосредственными клиентами.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1487,1018 +1118,35 @@
         <x:v>68</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:26">
-      <x:c r="A16" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B16" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C16" s="6" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="D16" s="5" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E16" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F16" s="5" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="G16" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H16" s="5" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="I16" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J16" s="5" t="s">
-        <x:v>75</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:26">
-      <x:c r="A17" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B17" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C17" s="6" t="s">
-        <x:v>76</x:v>
-      </x:c>
-      <x:c r="D17" s="5" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="E17" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F17" s="5" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="G17" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H17" s="5" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="I17" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J17" s="5" t="s">
-        <x:v>80</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:26">
-      <x:c r="A18" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B18" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C18" s="6" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="D18" s="5" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="E18" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F18" s="5" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="G18" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H18" s="5" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="I18" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J18" s="5" t="s">
-        <x:v>84</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:26">
-      <x:c r="A19" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B19" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C19" s="6" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="D19" s="5" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="E19" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F19" s="5" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="G19" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H19" s="5" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="I19" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J19" s="5" t="s"/>
-    </x:row>
-    <x:row r="20" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A20" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B20" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C20" s="6" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="D20" s="5" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="E20" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F20" s="5" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="G20" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H20" s="5" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="I20" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J20" s="5" t="s">
-        <x:v>91</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A21" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B21" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C21" s="6" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="D21" s="5" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="E21" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F21" s="5" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="G21" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H21" s="5" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="I21" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J21" s="5" t="s">
-        <x:v>95</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A22" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B22" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C22" s="6" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="D22" s="5" t="s">
-        <x:v>91</x:v>
-      </x:c>
-      <x:c r="E22" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F22" s="5" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="G22" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H22" s="5" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="I22" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J22" s="5" t="s"/>
-    </x:row>
-    <x:row r="23" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A23" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B23" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C23" s="6" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="D23" s="5" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E23" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F23" s="5" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="G23" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H23" s="5" t="s">
-        <x:v>102</x:v>
-      </x:c>
-      <x:c r="I23" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J23" s="5" t="s"/>
-    </x:row>
-    <x:row r="24" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A24" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B24" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C24" s="6" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="D24" s="5" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E24" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F24" s="5" t="s">
-        <x:v>104</x:v>
-      </x:c>
-      <x:c r="G24" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H24" s="5" t="s">
-        <x:v>105</x:v>
-      </x:c>
-      <x:c r="I24" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J24" s="5" t="s"/>
-    </x:row>
-    <x:row r="25" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A25" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B25" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C25" s="6" t="s">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="D25" s="5" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E25" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F25" s="5" t="s">
-        <x:v>107</x:v>
-      </x:c>
-      <x:c r="G25" s="5" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="H25" s="5" t="s">
-        <x:v>109</x:v>
-      </x:c>
-      <x:c r="I25" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J25" s="5" t="s"/>
-    </x:row>
-    <x:row r="26" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A26" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B26" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C26" s="6" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="D26" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E26" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F26" s="5" t="s">
-        <x:v>112</x:v>
-      </x:c>
-      <x:c r="G26" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H26" s="5" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="I26" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J26" s="5" t="s"/>
-    </x:row>
-    <x:row r="27" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A27" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B27" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C27" s="6" t="s">
-        <x:v>114</x:v>
-      </x:c>
-      <x:c r="D27" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E27" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F27" s="5" t="s">
-        <x:v>115</x:v>
-      </x:c>
-      <x:c r="G27" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H27" s="5" t="s">
-        <x:v>116</x:v>
-      </x:c>
-      <x:c r="I27" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J27" s="5" t="s"/>
-    </x:row>
-    <x:row r="28" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A28" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B28" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C28" s="6" t="s">
-        <x:v>117</x:v>
-      </x:c>
-      <x:c r="D28" s="5" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="E28" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F28" s="5" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="G28" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H28" s="5" t="s">
-        <x:v>120</x:v>
-      </x:c>
-      <x:c r="I28" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J28" s="5" t="s"/>
-    </x:row>
-    <x:row r="29" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A29" s="4" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B29" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C29" s="6" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="D29" s="5" t="s">
-        <x:v>91</x:v>
-      </x:c>
-      <x:c r="E29" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F29" s="5" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="G29" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H29" s="5" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="I29" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J29" s="5" t="s"/>
-    </x:row>
-    <x:row r="30" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A30" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B30" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C30" s="6" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="D30" s="5" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E30" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F30" s="5" t="s">
-        <x:v>126</x:v>
-      </x:c>
-      <x:c r="G30" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H30" s="5" t="s">
-        <x:v>127</x:v>
-      </x:c>
-      <x:c r="I30" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J30" s="5" t="s"/>
-    </x:row>
-    <x:row r="31" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A31" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B31" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C31" s="6" t="s">
-        <x:v>128</x:v>
-      </x:c>
-      <x:c r="D31" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E31" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F31" s="5" t="s">
-        <x:v>129</x:v>
-      </x:c>
-      <x:c r="G31" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H31" s="5" t="s">
-        <x:v>130</x:v>
-      </x:c>
-      <x:c r="I31" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J31" s="5" t="s"/>
-    </x:row>
-    <x:row r="32" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A32" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B32" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C32" s="6" t="s">
-        <x:v>131</x:v>
-      </x:c>
-      <x:c r="D32" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E32" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F32" s="5" t="s">
-        <x:v>132</x:v>
-      </x:c>
-      <x:c r="G32" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H32" s="5" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="I32" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J32" s="5" t="s"/>
-    </x:row>
-    <x:row r="33" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A33" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B33" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C33" s="6" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="D33" s="5" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E33" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F33" s="5" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="G33" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H33" s="5" t="s">
-        <x:v>136</x:v>
-      </x:c>
-      <x:c r="I33" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J33" s="5" t="s"/>
-    </x:row>
-    <x:row r="34" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A34" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B34" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C34" s="6" t="s">
-        <x:v>137</x:v>
-      </x:c>
-      <x:c r="D34" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E34" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F34" s="5" t="s">
-        <x:v>138</x:v>
-      </x:c>
-      <x:c r="G34" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H34" s="5" t="s">
-        <x:v>139</x:v>
-      </x:c>
-      <x:c r="I34" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J34" s="5" t="s">
-        <x:v>140</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A35" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B35" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C35" s="6" t="s">
-        <x:v>141</x:v>
-      </x:c>
-      <x:c r="D35" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E35" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F35" s="5" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="G35" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H35" s="5" t="s">
-        <x:v>143</x:v>
-      </x:c>
-      <x:c r="I35" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J35" s="5" t="s">
-        <x:v>144</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A36" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B36" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C36" s="6" t="s">
-        <x:v>145</x:v>
-      </x:c>
-      <x:c r="D36" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E36" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F36" s="5" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="G36" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H36" s="5" t="s">
-        <x:v>147</x:v>
-      </x:c>
-      <x:c r="I36" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J36" s="5" t="s">
-        <x:v>148</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A37" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B37" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C37" s="6" t="s">
-        <x:v>149</x:v>
-      </x:c>
-      <x:c r="D37" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E37" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F37" s="5" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="G37" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H37" s="5" t="s">
-        <x:v>151</x:v>
-      </x:c>
-      <x:c r="I37" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J37" s="5" t="s"/>
-    </x:row>
-    <x:row r="38" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A38" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B38" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C38" s="6" t="s">
-        <x:v>152</x:v>
-      </x:c>
-      <x:c r="D38" s="5" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E38" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F38" s="5" t="s">
-        <x:v>153</x:v>
-      </x:c>
-      <x:c r="G38" s="5" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="H38" s="5" t="s">
-        <x:v>154</x:v>
-      </x:c>
-      <x:c r="I38" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J38" s="5" t="s"/>
-    </x:row>
-    <x:row r="39" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A39" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B39" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C39" s="6" t="s">
-        <x:v>155</x:v>
-      </x:c>
-      <x:c r="D39" s="5" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="E39" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F39" s="5" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="G39" s="5" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="H39" s="5" t="s">
-        <x:v>157</x:v>
-      </x:c>
-      <x:c r="I39" s="5" t="s">
-        <x:v>158</x:v>
-      </x:c>
-      <x:c r="J39" s="5" t="s"/>
-    </x:row>
-    <x:row r="40" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A40" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B40" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C40" s="6" t="s">
-        <x:v>159</x:v>
-      </x:c>
-      <x:c r="D40" s="5" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="E40" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F40" s="5" t="s">
-        <x:v>160</x:v>
-      </x:c>
-      <x:c r="G40" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H40" s="5" t="s">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="I40" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J40" s="5" t="s">
-        <x:v>162</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A41" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="B41" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C41" s="6" t="s">
-        <x:v>163</x:v>
-      </x:c>
-      <x:c r="D41" s="5" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="E41" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F41" s="5" t="s">
-        <x:v>164</x:v>
-      </x:c>
-      <x:c r="G41" s="5" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="H41" s="5" t="s">
-        <x:v>165</x:v>
-      </x:c>
-      <x:c r="I41" s="5" t="s">
-        <x:v>158</x:v>
-      </x:c>
-      <x:c r="J41" s="5" t="s"/>
-    </x:row>
-    <x:row r="42" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A42" s="4" t="s">
-        <x:v>166</x:v>
-      </x:c>
-      <x:c r="B42" s="5" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="C42" s="6" t="s">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="D42" s="5" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="E42" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F42" s="5" t="s">
-        <x:v>169</x:v>
-      </x:c>
-      <x:c r="G42" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H42" s="5" t="s">
-        <x:v>170</x:v>
-      </x:c>
-      <x:c r="I42" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J42" s="5" t="s">
-        <x:v>171</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A43" s="4" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="B43" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C43" s="6" t="s">
-        <x:v>173</x:v>
-      </x:c>
-      <x:c r="D43" s="5" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="E43" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F43" s="5" t="s">
-        <x:v>174</x:v>
-      </x:c>
-      <x:c r="G43" s="5" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="H43" s="5" t="s">
-        <x:v>175</x:v>
-      </x:c>
-      <x:c r="I43" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J43" s="5" t="s"/>
-    </x:row>
-    <x:row r="44" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A44" s="4" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="B44" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C44" s="6" t="s">
-        <x:v>176</x:v>
-      </x:c>
-      <x:c r="D44" s="5" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="E44" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F44" s="5" t="s">
-        <x:v>177</x:v>
-      </x:c>
-      <x:c r="G44" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H44" s="5" t="s">
-        <x:v>178</x:v>
-      </x:c>
-      <x:c r="I44" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J44" s="5" t="s"/>
-    </x:row>
-    <x:row r="45" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A45" s="4" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="B45" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C45" s="6" t="s">
-        <x:v>179</x:v>
-      </x:c>
-      <x:c r="D45" s="5" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="E45" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F45" s="5" t="s">
-        <x:v>180</x:v>
-      </x:c>
-      <x:c r="G45" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H45" s="5" t="s">
-        <x:v>181</x:v>
-      </x:c>
-      <x:c r="I45" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J45" s="5" t="s"/>
-    </x:row>
-    <x:row r="46" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A46" s="4" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="B46" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C46" s="6" t="s">
-        <x:v>182</x:v>
-      </x:c>
-      <x:c r="D46" s="5" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="E46" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F46" s="5" t="s">
-        <x:v>183</x:v>
-      </x:c>
-      <x:c r="G46" s="5" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="H46" s="5" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="I46" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J46" s="5" t="s"/>
-    </x:row>
-    <x:row r="47" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A47" s="4" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="B47" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C47" s="6" t="s">
-        <x:v>185</x:v>
-      </x:c>
-      <x:c r="D47" s="5" t="s">
-        <x:v>186</x:v>
-      </x:c>
-      <x:c r="E47" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F47" s="5" t="s">
-        <x:v>187</x:v>
-      </x:c>
-      <x:c r="G47" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H47" s="5" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="I47" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J47" s="5" t="s"/>
-    </x:row>
-    <x:row r="48" spans="1:26" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A48" s="4" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="B48" s="5" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C48" s="6" t="s">
-        <x:v>189</x:v>
-      </x:c>
-      <x:c r="D48" s="5" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="E48" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F48" s="5" t="s">
-        <x:v>190</x:v>
-      </x:c>
-      <x:c r="G48" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H48" s="5" t="s">
-        <x:v>191</x:v>
-      </x:c>
-      <x:c r="I48" s="5" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J48" s="5" t="s">
-        <x:v>91</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="20" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="21" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="22" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="23" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="24" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="25" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="26" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="27" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="28" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="29" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="30" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="31" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="32" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="33" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="34" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="35" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="36" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="37" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="38" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="39" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="40" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="41" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="42" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="43" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="44" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="45" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="46" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="47" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
+    <x:row r="48" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
     <x:row r="49" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
     <x:row r="50" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
     <x:row r="51" spans="1:26" customFormat="1" ht="15.75" customHeight="1"/>
@@ -3470,39 +2118,6 @@
     <x:hyperlink ref="C13" r:id="rId37"/>
     <x:hyperlink ref="C14" r:id="rId38"/>
     <x:hyperlink ref="C15" r:id="rId39"/>
-    <x:hyperlink ref="C16" r:id="rId40"/>
-    <x:hyperlink ref="C17" r:id="rId41"/>
-    <x:hyperlink ref="C18" r:id="rId42"/>
-    <x:hyperlink ref="C19" r:id="rId43"/>
-    <x:hyperlink ref="C20" r:id="rId44"/>
-    <x:hyperlink ref="C21" r:id="rId45"/>
-    <x:hyperlink ref="C22" r:id="rId46"/>
-    <x:hyperlink ref="C23" r:id="rId47"/>
-    <x:hyperlink ref="C24" r:id="rId48"/>
-    <x:hyperlink ref="C25" r:id="rId49"/>
-    <x:hyperlink ref="C26" r:id="rId50"/>
-    <x:hyperlink ref="C27" r:id="rId51"/>
-    <x:hyperlink ref="C28" r:id="rId52"/>
-    <x:hyperlink ref="C29" r:id="rId53"/>
-    <x:hyperlink ref="C30" r:id="rId54"/>
-    <x:hyperlink ref="C31" r:id="rId55"/>
-    <x:hyperlink ref="C32" r:id="rId56"/>
-    <x:hyperlink ref="C33" r:id="rId57"/>
-    <x:hyperlink ref="C34" r:id="rId58"/>
-    <x:hyperlink ref="C35" r:id="rId59"/>
-    <x:hyperlink ref="C36" r:id="rId60"/>
-    <x:hyperlink ref="C37" r:id="rId61"/>
-    <x:hyperlink ref="C38" r:id="rId62"/>
-    <x:hyperlink ref="C39" r:id="rId63"/>
-    <x:hyperlink ref="C40" r:id="rId64"/>
-    <x:hyperlink ref="C41" r:id="rId65"/>
-    <x:hyperlink ref="C42" r:id="rId66"/>
-    <x:hyperlink ref="C43" r:id="rId67"/>
-    <x:hyperlink ref="C44" r:id="rId68"/>
-    <x:hyperlink ref="C45" r:id="rId69"/>
-    <x:hyperlink ref="C46" r:id="rId70"/>
-    <x:hyperlink ref="C47" r:id="rId71"/>
-    <x:hyperlink ref="C48" r:id="rId72"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0" footer="0"/>

</xml_diff>